<commit_message>
trying to clear up error when loading tab_49 reports
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_49_rpt_PF_NetRecoveries.xlsx
+++ b/backend/reports/xlsx/Tab_49_rpt_PF_NetRecoveries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acarmich\source\repos\gdx-agreements-tracker\backend\reports\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A3CBDAC-A22E-8B46-BA9F-5B41DDB538CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306A4086-97CC-411A-AA1B-D7F3581E3F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,30 +36,100 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>{#r=d.report[i]}</t>
-  </si>
-  <si>
-    <t>{#r1=d.report[i+1]}</t>
-  </si>
-  <si>
-    <t>{#t=d.report_totals[i]}</t>
-  </si>
-  <si>
-    <t>{#date=d.date}</t>
-  </si>
-  <si>
-    <t>Project #</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
-    <t>{#fy=d.fiscal_year}</t>
-  </si>
-  <si>
-    <t>Project ________ for {$fy} as of {$date}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t>{#r = d.report[i]}</t>
+  </si>
+  <si>
+    <t>{#r1= d.report[i+1]}</t>
+  </si>
+  <si>
+    <t>{#rp = d.report[i].projects[i]}</t>
+  </si>
+  <si>
+    <t>{#rp1 = d.report[i].projects[i+1]}</t>
+  </si>
+  <si>
+    <t>{#rt = d.report[i].portfolio_totals}</t>
+  </si>
+  <si>
+    <t>{$rt.totals_recoveries}</t>
+  </si>
+  <si>
+    <t>{$rt.totals_net}</t>
+  </si>
+  <si>
+    <t>{$rt.totals_to_date}</t>
+  </si>
+  <si>
+    <t>{$rt.totals_remaining}</t>
+  </si>
+  <si>
+    <t>{$r.portfolio_name}</t>
+  </si>
+  <si>
+    <t>Total Recoveries For Projects</t>
+  </si>
+  <si>
+    <t>Less All Project Expenses</t>
+  </si>
+  <si>
+    <t>Net Recoveries</t>
+  </si>
+  <si>
+    <t>Recovered To Date</t>
+  </si>
+  <si>
+    <t>Remaining Recoveries</t>
+  </si>
+  <si>
+    <t>{$rp.project_number}</t>
+  </si>
+  <si>
+    <t>{$rp.project_name}</t>
+  </si>
+  <si>
+    <t>{$rp.total_recoverable}</t>
+  </si>
+  <si>
+    <t>{$rp.less_expenses}</t>
+  </si>
+  <si>
+    <t>{$rp.net_recoveries}</t>
+  </si>
+  <si>
+    <t>{$rp.recovered_to_date}</t>
+  </si>
+  <si>
+    <t>{$rp.remaining_recoveries}</t>
+  </si>
+  <si>
+    <t>{$rp1.project_number}</t>
+  </si>
+  <si>
+    <t>{$r.portfolio_name} Total:</t>
+  </si>
+  <si>
+    <t>{$rt.totals_expenses}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="0"/>
+        <rFont val="BCSans-Regular"/>
+      </rPr>
+      <t xml:space="preserve">GDX Project Net Recoveries Report as of {d.date} 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="BCSans-Regular"/>
+      </rPr>
+      <t xml:space="preserve">Fiscal Year: {d.fiscal}, Portfolio(s): </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -69,7 +139,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,11 +152,6 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
       <sz val="8.5"/>
       <name val="BCSans-Regular"/>
     </font>
@@ -101,12 +166,81 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8.5"/>
+      <color rgb="FF000000"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8.5"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="8.5"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="BCSans-Regular"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="BC Sans"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,8 +259,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD6EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -160,19 +324,6 @@
       <bottom style="medium">
         <color rgb="FFBFBFBF"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA5A5A5"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -185,6 +336,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color rgb="FFBFBFBF"/>
@@ -192,6 +382,41 @@
       <top style="medium">
         <color rgb="FFBFBFBF"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FFBFBFBF"/>
       </bottom>
@@ -201,49 +426,118 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -324,9 +618,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -364,7 +658,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -470,7 +764,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -612,7 +906,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -623,112 +917,205 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I2" sqref="C2:I2"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="9" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="11.19921875" customWidth="1"/>
+    <col min="2" max="2" width="43.19921875" customWidth="1"/>
+    <col min="3" max="7" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="22"/>
+      <c r="B3" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="32"/>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="4"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="32"/>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="3"/>
+      <c r="B7" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="7" t="s">
+      <c r="G7" s="40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
+    </row>
+    <row r="20" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="13"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="A19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Some work on the template
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_49_rpt_PF_NetRecoveries.xlsx
+++ b/backend/reports/xlsx/Tab_49_rpt_PF_NetRecoveries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acarmich\source\repos\gdx-agreements-tracker\backend\reports\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9483A7B0-3958-4048-8E90-1E2C02ADE754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F252EA8-4941-4E8F-B95D-9671B18509BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>{#r = d.report[i]}</t>
   </si>
@@ -86,15 +86,75 @@
       <t xml:space="preserve">Fiscal Year: {d.fiscal}, Portfolio(s): </t>
     </r>
   </si>
+  <si>
+    <t>{$r.portfolio_name}</t>
+  </si>
+  <si>
+    <t>{$rp.project_number}</t>
+  </si>
+  <si>
+    <t>{$rp.project_name}</t>
+  </si>
+  <si>
+    <t>{$rp.total_recoverable}</t>
+  </si>
+  <si>
+    <t>{$rp.less_expenses}</t>
+  </si>
+  <si>
+    <t>{$rp.net_recoveries}</t>
+  </si>
+  <si>
+    <t>{$rp.recovered_to_date}</t>
+  </si>
+  <si>
+    <t>{$rp.remaining_recoveries}</t>
+  </si>
+  <si>
+    <t>{$rp1.project_number}</t>
+  </si>
+  <si>
+    <t>{$r.portfolio_name} Total:</t>
+  </si>
+  <si>
+    <t>{$rt.totals_recoveries}</t>
+  </si>
+  <si>
+    <t>{$rt.totals_expenses}</t>
+  </si>
+  <si>
+    <t>{$rt.totals_net}</t>
+  </si>
+  <si>
+    <t>{$rt.totals_to_date}</t>
+  </si>
+  <si>
+    <t>{$rt.totals_remaining}</t>
+  </si>
+  <si>
+    <t>{$r1.portfolio_name}</t>
+  </si>
+  <si>
+    <t>GDX Division Summary</t>
+  </si>
+  <si>
+    <t>{$r.portfolio_name}:</t>
+  </si>
+  <si>
+    <t>{$r1.portfolio_name}:</t>
+  </si>
+  <si>
+    <t>TOTAL:</t>
+  </si>
+  <si>
+    <t>{$rt. totals_expenses}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-  </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,15 +167,6 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <sz val="8.5"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="0"/>
       <name val="BCSans-Regular"/>
@@ -127,72 +178,89 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8.5"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="8.5"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8.5"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8.5"/>
-      <color rgb="FF000000"/>
-      <name val="BC Sans"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="BC Sans"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="BC Sans"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="BC Sans"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8.5"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="BC Sans"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="0"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="0"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <sz val="8.5"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="BC Sans"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="BC Sans"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="BC Sans"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="BC Sans"/>
     </font>
   </fonts>
   <fills count="9">
@@ -234,18 +302,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor rgb="FFE7E6E6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE7E6E6"/>
+        <fgColor rgb="FFAEAAAA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -254,23 +322,75 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFA5A5A5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color rgb="FFBFBFBF"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FFBFBFBF"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color rgb="FFBFBFBF"/>
-      </top>
+      </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FFBFBFBF"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="medium">
         <color rgb="FFBFBFBF"/>
@@ -282,98 +402,111 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color rgb="FFA5A5A5"/>
+        <color rgb="FFBFBFBF"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="medium">
         <color rgb="FFBFBFBF"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -381,118 +514,132 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -872,175 +1019,221 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="A3:H8"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.19921875" customWidth="1"/>
-    <col min="2" max="2" width="43.19921875" customWidth="1"/>
-    <col min="3" max="7" width="15.796875" customWidth="1"/>
+    <col min="2" max="2" width="43.19921875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" style="15" customWidth="1"/>
+    <col min="4" max="7" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="11" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="31" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" s="23" customFormat="1" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="21" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="22"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="23"/>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="33"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="35"/>
-    </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="38"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="32"/>
-    </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="4"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="32"/>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="3"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="40"/>
+      <c r="A3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.4">
+      <c r="A5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
+    </row>
+    <row r="6" spans="1:7" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A6" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
+      <c r="A9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
+      <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="21"/>
-    </row>
-    <row r="20" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-    </row>
-    <row r="21" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="13"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-    </row>
-    <row r="22" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
+    <row r="15" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+    </row>
+    <row r="16" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="37"/>
+      <c r="C16" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="37"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="43"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="38"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="43"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="9">
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A15:G15"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
-    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
fixed up some formatting issues.
Looks great!
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_49_rpt_PF_NetRecoveries.xlsx
+++ b/backend/reports/xlsx/Tab_49_rpt_PF_NetRecoveries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acarmich\source\repos\gdx-agreements-tracker\backend\reports\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD15531-530A-4D90-9764-AC7CEC73F432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4C9AE3-BE14-4C71-AB71-5FE4FAAD42BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -68,6 +68,87 @@
     <t>Remaining Recoveries</t>
   </si>
   <si>
+    <t>{$r.portfolio_name}</t>
+  </si>
+  <si>
+    <t>{$rp.project_number}</t>
+  </si>
+  <si>
+    <t>{$rp.project_name}</t>
+  </si>
+  <si>
+    <t>{$rp.total_recoverable}</t>
+  </si>
+  <si>
+    <t>{$rp.less_expenses}</t>
+  </si>
+  <si>
+    <t>{$rp.net_recoveries}</t>
+  </si>
+  <si>
+    <t>{$rp.recovered_to_date}</t>
+  </si>
+  <si>
+    <t>{$rp.remaining_recoveries}</t>
+  </si>
+  <si>
+    <t>{$rp1.project_number}</t>
+  </si>
+  <si>
+    <t>{$r.portfolio_name} Total:</t>
+  </si>
+  <si>
+    <t>{$rt.totals_recoveries}</t>
+  </si>
+  <si>
+    <t>{$rt.totals_expenses}</t>
+  </si>
+  <si>
+    <t>{$rt.totals_net}</t>
+  </si>
+  <si>
+    <t>{$rt.totals_to_date}</t>
+  </si>
+  <si>
+    <t>{$rt.totals_remaining}</t>
+  </si>
+  <si>
+    <t>{$r1.portfolio_name}</t>
+  </si>
+  <si>
+    <t>GDX Division Summary</t>
+  </si>
+  <si>
+    <t>{$r.portfolio_name}:</t>
+  </si>
+  <si>
+    <t>{$r1.portfolio_name}:</t>
+  </si>
+  <si>
+    <t>TOTAL:</t>
+  </si>
+  <si>
+    <t>{$rt. totals_expenses}</t>
+  </si>
+  <si>
+    <t>{#gt = d.grand_totals}</t>
+  </si>
+  <si>
+    <t>{$gt.totals_recoveries_sum}</t>
+  </si>
+  <si>
+    <t>{$gt.totals_expenses_sum}</t>
+  </si>
+  <si>
+    <t>{$gt.totals_net_sum}</t>
+  </si>
+  <si>
+    <t>{$gt.totals_to_date_sum}</t>
+  </si>
+  <si>
+    <t>{$gt.totals_remaining_sum}</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="16"/>
@@ -83,89 +164,8 @@
         <color theme="0"/>
         <rFont val="BCSans-Regular"/>
       </rPr>
-      <t xml:space="preserve">Fiscal Year: {d.fiscal}, Portfolio(s): </t>
+      <t>Fiscal Year: {d.fiscal}</t>
     </r>
-  </si>
-  <si>
-    <t>{$r.portfolio_name}</t>
-  </si>
-  <si>
-    <t>{$rp.project_number}</t>
-  </si>
-  <si>
-    <t>{$rp.project_name}</t>
-  </si>
-  <si>
-    <t>{$rp.total_recoverable}</t>
-  </si>
-  <si>
-    <t>{$rp.less_expenses}</t>
-  </si>
-  <si>
-    <t>{$rp.net_recoveries}</t>
-  </si>
-  <si>
-    <t>{$rp.recovered_to_date}</t>
-  </si>
-  <si>
-    <t>{$rp.remaining_recoveries}</t>
-  </si>
-  <si>
-    <t>{$rp1.project_number}</t>
-  </si>
-  <si>
-    <t>{$r.portfolio_name} Total:</t>
-  </si>
-  <si>
-    <t>{$rt.totals_recoveries}</t>
-  </si>
-  <si>
-    <t>{$rt.totals_expenses}</t>
-  </si>
-  <si>
-    <t>{$rt.totals_net}</t>
-  </si>
-  <si>
-    <t>{$rt.totals_to_date}</t>
-  </si>
-  <si>
-    <t>{$rt.totals_remaining}</t>
-  </si>
-  <si>
-    <t>{$r1.portfolio_name}</t>
-  </si>
-  <si>
-    <t>GDX Division Summary</t>
-  </si>
-  <si>
-    <t>{$r.portfolio_name}:</t>
-  </si>
-  <si>
-    <t>{$r1.portfolio_name}:</t>
-  </si>
-  <si>
-    <t>TOTAL:</t>
-  </si>
-  <si>
-    <t>{$rt. totals_expenses}</t>
-  </si>
-  <si>
-    <t>{#gt = d.grand_totals}</t>
-  </si>
-  <si>
-    <t>{$gt.totals_recoveries_sum}</t>
-  </si>
-  <si>
-    <t>{$gt.totals_expenses_sum}</t>
-  </si>
-  <si>
-    <t>{$gt.totals_net_sum}</t>
-  </si>
-  <si>
-    <t>{$gt.totals_to_date_sum}</t>
-  </si>
-  <si>
-    <t>{$gt.totals_remaining_sum}</t>
   </si>
 </sst>
 </file>
@@ -281,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,18 +320,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE7E6E6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFAEAAAA"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -426,7 +420,27 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -436,7 +450,7 @@
       </left>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -505,6 +519,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -522,6 +547,86 @@
       <right/>
       <top style="thin">
         <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
@@ -532,135 +637,148 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1040,233 +1158,262 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.19921875" customWidth="1"/>
-    <col min="2" max="2" width="43.19921875" style="15" customWidth="1"/>
-    <col min="3" max="3" width="15.796875" style="15" customWidth="1"/>
-    <col min="4" max="7" width="15.796875" customWidth="1"/>
+    <col min="1" max="1" width="11.19921875" style="33" customWidth="1"/>
+    <col min="2" max="2" width="43.19921875" style="33" customWidth="1"/>
+    <col min="3" max="7" width="15.796875" style="33" customWidth="1"/>
+    <col min="8" max="16384" width="11.19921875" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" s="16" customFormat="1" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:7" s="23" customFormat="1" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="12" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="36"/>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="13" t="s">
+      <c r="B4" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="C4" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.4">
+      <c r="A5" s="17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.4">
-      <c r="A5" s="24" t="s">
+      <c r="B5" s="38"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="29"/>
+    </row>
+    <row r="6" spans="1:7" s="20" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A6" s="45"/>
+      <c r="B6" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
-    </row>
-    <row r="6" spans="1:7" s="32" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.4">
-      <c r="A6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="30" t="s">
+      <c r="D6" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="E6" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="F6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="G6" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="30" t="s">
+    </row>
+    <row r="7" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="39" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+    </row>
+    <row r="8" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="33"/>
+    </row>
+    <row r="9" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="33"/>
+    </row>
+    <row r="10" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="33"/>
+    </row>
+    <row r="11" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="33"/>
+    </row>
+    <row r="12" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="33"/>
+    </row>
+    <row r="13" spans="1:7" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="51" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+    </row>
+    <row r="14" spans="1:7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="47"/>
+      <c r="B14" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="23"/>
+    </row>
+    <row r="16" spans="1:7" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="48"/>
+      <c r="B16" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="25" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-    </row>
-    <row r="16" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+    </row>
+    <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="42" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="41"/>
-    </row>
-    <row r="18" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="46" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+    </row>
+    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+    </row>
+    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="33"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+    </row>
+    <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="33"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+    </row>
+    <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A18:B18"/>
+  <mergeCells count="5">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A13:G13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
suggested fixed for report
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_49_rpt_PF_NetRecoveries.xlsx
+++ b/backend/reports/xlsx/Tab_49_rpt_PF_NetRecoveries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aspiteri/Development/Github/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B22890-8E93-A14F-A5D9-6A6FA399F3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC7D63D-104E-BA4B-BC95-F79F9C8AFBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26640" activeTab="1" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="26640" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Net Recoveries" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>{#r = d.report[i]}</t>
   </si>
@@ -150,30 +150,18 @@
     <t>{$gt.totals_remaining_sum}</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="0"/>
-        <rFont val="BCSans-Regular"/>
-      </rPr>
-      <t xml:space="preserve">GDX Project Net Recoveries Report as of {d.date} 
+    <t xml:space="preserve">GDX Project Net Recoveries Report as of {d.date} 
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="BCSans-Regular"/>
-      </rPr>
-      <t>Fiscal Year: {d.fiscal}</t>
-    </r>
+  </si>
+  <si>
+    <t>Fiscal Year: {d.fiscal};  Portfolio(s): {d.portfolios.portfolioNames} ;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -206,17 +194,6 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="BC Sans"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8.5"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="BC Sans"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="0"/>
-      <name val="BCSans-Regular"/>
     </font>
     <font>
       <sz val="16"/>
@@ -274,6 +251,11 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="BCSans-Regular"/>
     </font>
   </fonts>
   <fills count="8">
@@ -320,7 +302,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -626,6 +608,15 @@
       <bottom style="medium">
         <color rgb="FFBFBFBF"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFA5A5A5"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -639,22 +630,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -664,7 +655,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -673,106 +664,79 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
@@ -780,15 +744,42 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,15 +808,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>407175</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1561691</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>680356</xdr:rowOff>
+      <xdr:colOff>1240120</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>155114</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -854,8 +845,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2411054" cy="680356"/>
+          <a:off x="407175" y="0"/>
+          <a:ext cx="1686075" cy="475038"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1167,11 +1158,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView zoomScale="131" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10:H16"/>
+    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" outlineLevelCol="1"/>
@@ -1180,156 +1171,164 @@
     <col min="2" max="2" width="43.1640625" customWidth="1"/>
     <col min="3" max="6" width="15.83203125" customWidth="1"/>
     <col min="7" max="7" width="20.5" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" style="56" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="11.1640625" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="31" t="s">
+    <row r="1" spans="1:9" ht="25" customHeight="1" thickBot="1">
+      <c r="A1" s="47"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="53"/>
-    </row>
-    <row r="2" spans="1:9" s="8" customFormat="1" ht="34" customHeight="1" thickBot="1">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="4" t="s">
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+    </row>
+    <row r="2" spans="1:9" s="57" customFormat="1" ht="20" customHeight="1">
+      <c r="A2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+    </row>
+    <row r="3" spans="1:9" s="8" customFormat="1" ht="34" customHeight="1" thickBot="1">
+      <c r="A3" s="45"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="54"/>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="19.75" customHeight="1">
-      <c r="A3" s="33" t="s">
+      <c r="H3" s="44"/>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="19.75" customHeight="1">
+      <c r="A4" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="53"/>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="33" thickBot="1">
-      <c r="A4" s="36" t="s">
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="51"/>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="33" thickBot="1">
+      <c r="A5" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E5" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F5" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G5" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="53"/>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="32">
-      <c r="A5" s="41" t="s">
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="32">
+      <c r="A6" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="55"/>
-    </row>
-    <row r="6" spans="1:9" s="10" customFormat="1" ht="19">
-      <c r="A6" s="21"/>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="38"/>
+    </row>
+    <row r="7" spans="1:9" s="10" customFormat="1" ht="19">
+      <c r="A7" s="21"/>
+      <c r="B7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G7" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="55"/>
-      <c r="I6" s="52"/>
-    </row>
-    <row r="7" spans="1:9" ht="17">
-      <c r="A7" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="17">
-      <c r="H10" s="57" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="43"/>
+    </row>
+    <row r="8" spans="1:9" ht="17">
+      <c r="A8" s="3"/>
+    </row>
+    <row r="11" spans="1:9" ht="17">
+      <c r="H11" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17">
-      <c r="H11" s="57" t="s">
+    <row r="12" spans="1:9" ht="17">
+      <c r="H12" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17">
-      <c r="H12" s="57" t="s">
+    <row r="13" spans="1:9" ht="17">
+      <c r="H13" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17">
-      <c r="H13" s="57" t="s">
+    <row r="14" spans="1:9" ht="17">
+      <c r="H14" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17">
-      <c r="H14" s="57" t="s">
+    <row r="15" spans="1:9" ht="17">
+      <c r="H15" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="17">
-      <c r="H15" s="57" t="s">
+    <row r="16" spans="1:9" ht="17">
+      <c r="H16" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17">
-      <c r="H16" s="57" t="s">
+    <row r="17" spans="8:8" ht="17">
+      <c r="H17" s="3" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:B2"/>
+  <mergeCells count="5">
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
-    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="C2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -1345,7 +1344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D26818D4-5613-4749-A554-D04D5CCBA2DB}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -1357,15 +1356,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="23"/>
@@ -1384,7 +1383,7 @@
       <c r="F2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="40" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1397,7 +1396,7 @@
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="50"/>
+      <c r="G3" s="41"/>
     </row>
     <row r="4" spans="1:10" ht="32">
       <c r="A4" s="24"/>
@@ -1416,42 +1415,42 @@
       <c r="F4" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="42" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="17">
-      <c r="J7" s="57" t="s">
+      <c r="J7" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="17">
-      <c r="J8" s="57" t="s">
+      <c r="J8" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="17">
-      <c r="J9" s="57" t="s">
+      <c r="J9" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="17">
-      <c r="J10" s="57" t="s">
+      <c r="J10" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="17">
-      <c r="J11" s="57" t="s">
+      <c r="J11" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="17">
-      <c r="J12" s="57" t="s">
+      <c r="J12" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="17">
-      <c r="J13" s="57" t="s">
+      <c r="J13" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed formatting issues in excel document
and fixed lint errors
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_49_rpt_PF_NetRecoveries.xlsx
+++ b/backend/reports/xlsx/Tab_49_rpt_PF_NetRecoveries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aspiteri/Development/Github/gdx-agreements-tracker/backend/reports/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acarmich\source\repos\gdx-agreements-tracker\backend\reports\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC7D63D-104E-BA4B-BC95-F79F9C8AFBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A840953-2E9B-4B74-BACF-36A1AAF927E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="26640" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Net Recoveries" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>{#r = d.report[i]}</t>
   </si>
@@ -161,7 +161,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -210,11 +210,6 @@
       <b/>
       <sz val="8"/>
       <color rgb="FF000000"/>
-      <name val="BC Sans"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8.5"/>
       <name val="BC Sans"/>
     </font>
     <font>
@@ -256,6 +251,11 @@
       <sz val="8"/>
       <color theme="0"/>
       <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="BC Sans"/>
     </font>
   </fonts>
   <fills count="8">
@@ -302,21 +302,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="25">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFA5A5A5"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -559,19 +550,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -610,176 +588,166 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFA5A5A5"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,7 +782,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1240120</xdr:colOff>
+      <xdr:colOff>1597674</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>155114</xdr:rowOff>
     </xdr:to>
@@ -1158,47 +1126,47 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:AH13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="6" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="6.5" customWidth="1"/>
+    <col min="2" max="2" width="43.19921875" customWidth="1"/>
+    <col min="3" max="6" width="15.796875" customWidth="1"/>
     <col min="7" max="7" width="20.5" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="11.19921875" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25" customHeight="1" thickBot="1">
-      <c r="A1" s="47"/>
-      <c r="B1" s="47"/>
-      <c r="C1" s="55" t="s">
+    <row r="1" spans="1:34" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-    </row>
-    <row r="2" spans="1:9" s="57" customFormat="1" ht="20" customHeight="1">
-      <c r="A2" s="52"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="54" t="s">
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+    </row>
+    <row r="2" spans="1:34" s="45" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-    </row>
-    <row r="3" spans="1:9" s="8" customFormat="1" ht="34" customHeight="1" thickBot="1">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+    </row>
+    <row r="3" spans="1:34" s="8" customFormat="1" ht="34.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="46"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1214,20 +1182,73 @@
       <c r="G3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="44"/>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="19.75" customHeight="1">
-      <c r="A4" s="48" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="53"/>
+      <c r="X3" s="53"/>
+      <c r="Y3" s="53"/>
+      <c r="Z3" s="53"/>
+      <c r="AA3" s="53"/>
+      <c r="AB3" s="53"/>
+      <c r="AC3" s="53"/>
+      <c r="AD3" s="53"/>
+      <c r="AE3" s="53"/>
+      <c r="AF3" s="53"/>
+      <c r="AG3" s="53"/>
+      <c r="AH3" s="53"/>
+    </row>
+    <row r="4" spans="1:34" s="1" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="57"/>
+      <c r="B4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="33" thickBot="1">
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="54"/>
+      <c r="T4" s="54"/>
+      <c r="U4" s="54"/>
+      <c r="V4" s="54"/>
+      <c r="W4" s="54"/>
+      <c r="X4" s="54"/>
+      <c r="Y4" s="54"/>
+      <c r="Z4" s="54"/>
+      <c r="AA4" s="54"/>
+      <c r="AB4" s="54"/>
+      <c r="AC4" s="54"/>
+      <c r="AD4" s="54"/>
+      <c r="AE4" s="54"/>
+      <c r="AF4" s="54"/>
+      <c r="AG4" s="54"/>
+      <c r="AH4" s="54"/>
+    </row>
+    <row r="5" spans="1:34" s="1" customFormat="1" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="27" t="s">
         <v>11</v>
       </c>
@@ -1249,8 +1270,35 @@
       <c r="G5" s="37" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="32">
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="54"/>
+      <c r="S5" s="54"/>
+      <c r="T5" s="54"/>
+      <c r="U5" s="54"/>
+      <c r="V5" s="54"/>
+      <c r="W5" s="54"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="54"/>
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="54"/>
+      <c r="AB5" s="54"/>
+      <c r="AC5" s="54"/>
+      <c r="AD5" s="54"/>
+      <c r="AE5" s="54"/>
+      <c r="AF5" s="54"/>
+      <c r="AG5" s="54"/>
+      <c r="AH5" s="54"/>
+    </row>
+    <row r="6" spans="1:34" s="2" customFormat="1" ht="26.4" x14ac:dyDescent="0.4">
       <c r="A6" s="32" t="s">
         <v>18</v>
       </c>
@@ -1260,8 +1308,35 @@
       <c r="E6" s="36"/>
       <c r="F6" s="35"/>
       <c r="G6" s="38"/>
-    </row>
-    <row r="7" spans="1:9" s="10" customFormat="1" ht="19">
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="55"/>
+      <c r="O6" s="55"/>
+      <c r="P6" s="55"/>
+      <c r="Q6" s="55"/>
+      <c r="R6" s="55"/>
+      <c r="S6" s="55"/>
+      <c r="T6" s="55"/>
+      <c r="U6" s="55"/>
+      <c r="V6" s="55"/>
+      <c r="W6" s="55"/>
+      <c r="X6" s="55"/>
+      <c r="Y6" s="55"/>
+      <c r="Z6" s="55"/>
+      <c r="AA6" s="55"/>
+      <c r="AB6" s="55"/>
+      <c r="AC6" s="55"/>
+      <c r="AD6" s="55"/>
+      <c r="AE6" s="55"/>
+      <c r="AF6" s="55"/>
+      <c r="AG6" s="55"/>
+      <c r="AH6" s="55"/>
+    </row>
+    <row r="7" spans="1:34" s="10" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
       <c r="B7" s="20" t="s">
         <v>19</v>
@@ -1281,53 +1356,81 @@
       <c r="G7" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="43"/>
-    </row>
-    <row r="8" spans="1:9" ht="17">
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="55"/>
+      <c r="Q7" s="55"/>
+      <c r="R7" s="55"/>
+      <c r="S7" s="55"/>
+      <c r="T7" s="55"/>
+      <c r="U7" s="55"/>
+      <c r="V7" s="55"/>
+      <c r="W7" s="55"/>
+      <c r="X7" s="55"/>
+      <c r="Y7" s="55"/>
+      <c r="Z7" s="55"/>
+      <c r="AA7" s="55"/>
+      <c r="AB7" s="55"/>
+      <c r="AC7" s="55"/>
+      <c r="AD7" s="55"/>
+      <c r="AE7" s="55"/>
+      <c r="AF7" s="55"/>
+      <c r="AG7" s="55"/>
+      <c r="AH7" s="55"/>
+    </row>
+    <row r="8" spans="1:34" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
-    </row>
-    <row r="11" spans="1:9" ht="17">
+      <c r="H8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="X8" s="56"/>
+      <c r="Y8" s="56"/>
+      <c r="Z8" s="56"/>
+      <c r="AA8" s="56"/>
+      <c r="AB8" s="56"/>
+      <c r="AC8" s="56"/>
+      <c r="AD8" s="56"/>
+      <c r="AE8" s="56"/>
+      <c r="AF8" s="56"/>
+      <c r="AG8" s="56"/>
+      <c r="AH8" s="56"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="H9" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="H10" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="H11" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="H12" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="H13" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="17">
-      <c r="H14" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="17">
-      <c r="H15" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="17">
-      <c r="H16" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" ht="17">
-      <c r="H17" s="3" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
-    <mergeCell ref="A4:G4"/>
     <mergeCell ref="C2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1348,25 +1451,25 @@
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="7" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="11.19921875" customWidth="1"/>
+    <col min="2" max="2" width="43.19921875" customWidth="1"/>
+    <col min="3" max="7" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="23"/>
       <c r="B2" s="22" t="s">
         <v>27</v>
@@ -1387,7 +1490,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
       <c r="B3" s="25" t="s">
         <v>28</v>
@@ -1398,7 +1501,7 @@
       <c r="F3" s="12"/>
       <c r="G3" s="41"/>
     </row>
-    <row r="4" spans="1:10" ht="32">
+    <row r="4" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A4" s="24"/>
       <c r="B4" s="26" t="s">
         <v>29</v>
@@ -1419,37 +1522,37 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J7" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J8" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="17">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J9" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="17">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J10" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J11" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="17">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J12" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J13" s="3" t="s">
         <v>4</v>
       </c>

</xml_diff>